<commit_message>
Add offline Ajv validator and switch to local script for offline JSON schema validation
Changed files:
- function/ajv7.min.js: added minified Ajv stub for offline use (replace with full code for production)
- start.html: switched Ajv script source from CDN to local file for offline/off-grid use
</commit_message>
<xml_diff>
--- a/original-excel-sources/budget-jodine-2025-2026.xlsx
+++ b/original-excel-sources/budget-jodine-2025-2026.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jay/GIT-Repos-Personal/ftrack/source files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jay/GIT-Repos-Personal/ftrack/original-excel-sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5188C738-7A5E-4542-B405-A038696019AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E69DF5-B425-0145-B599-D3122F468C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-137600" yWindow="-10980" windowWidth="68800" windowHeight="28300" activeTab="5" xr2:uid="{E4FDB97B-DCD0-C941-AC1E-362D6582387C}"/>
+    <workbookView xWindow="-68800" yWindow="-10980" windowWidth="68800" windowHeight="28300" activeTab="5" xr2:uid="{E4FDB97B-DCD0-C941-AC1E-362D6582387C}"/>
   </bookViews>
   <sheets>
     <sheet name="Jodine Main" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="159">
   <si>
     <t>Expense</t>
   </si>
@@ -535,7 +535,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -573,6 +573,12 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
@@ -685,7 +691,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -711,6 +717,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13690,8 +13697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24C67FA7-03EF-D349-9E43-C752CAA64204}">
   <dimension ref="A1:BJ26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="113" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="AF20" sqref="AF20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13703,7 +13710,8 @@
     <col min="5" max="5" width="7" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="9.1640625" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.5" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.5" bestFit="1" customWidth="1"/>
@@ -14026,7 +14034,7 @@
         <f>$B$9</f>
         <v>5000</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="23">
         <f t="shared" ref="I13:BJ13" si="0">$B$9</f>
         <v>5000</v>
       </c>
@@ -14264,9 +14272,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I14" s="18">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="I14" s="23">
+        <v>500</v>
       </c>
       <c r="J14" s="18">
         <f>$B$10</f>
@@ -14645,220 +14652,219 @@
         <v>21812.75</v>
       </c>
       <c r="I17" s="18">
-        <f t="shared" si="2"/>
-        <v>21858.19</v>
+        <v>21881.95</v>
       </c>
       <c r="J17" s="18">
         <f t="shared" si="2"/>
-        <v>22895.79</v>
+        <v>23420.639999999999</v>
       </c>
       <c r="K17" s="18">
         <f t="shared" si="2"/>
-        <v>23935.55</v>
+        <v>24461.5</v>
       </c>
       <c r="L17" s="18">
         <f t="shared" si="2"/>
-        <v>24977.48</v>
+        <v>25504.52</v>
       </c>
       <c r="M17" s="18">
         <f t="shared" si="2"/>
-        <v>26021.58</v>
+        <v>26549.72</v>
       </c>
       <c r="N17" s="18">
         <f t="shared" si="2"/>
-        <v>27067.85</v>
+        <v>27597.09</v>
       </c>
       <c r="O17" s="18">
         <f t="shared" si="2"/>
-        <v>28116.3</v>
+        <v>28646.65</v>
       </c>
       <c r="P17" s="18">
         <f>O24</f>
-        <v>21160.29</v>
+        <v>21691.75</v>
       </c>
       <c r="Q17" s="18">
         <f t="shared" si="2"/>
-        <v>21204.37</v>
+        <v>21736.94</v>
       </c>
       <c r="R17" s="18">
         <f t="shared" si="2"/>
-        <v>21248.55</v>
+        <v>21782.23</v>
       </c>
       <c r="S17" s="18">
         <f t="shared" si="2"/>
-        <v>21292.82</v>
+        <v>21827.61</v>
       </c>
       <c r="T17" s="18">
         <f t="shared" si="2"/>
-        <v>21337.18</v>
+        <v>21873.08</v>
       </c>
       <c r="U17" s="18">
         <f t="shared" si="2"/>
-        <v>21381.63</v>
+        <v>21918.65</v>
       </c>
       <c r="V17" s="18">
         <f t="shared" si="2"/>
-        <v>14411.59</v>
+        <v>14949.73</v>
       </c>
       <c r="W17" s="18">
         <f t="shared" si="2"/>
-        <v>14441.61</v>
+        <v>14980.88</v>
       </c>
       <c r="X17" s="18">
         <f t="shared" si="2"/>
-        <v>14471.7</v>
+        <v>15012.09</v>
       </c>
       <c r="Y17" s="18">
         <f t="shared" si="2"/>
-        <v>14501.85</v>
+        <v>15043.37</v>
       </c>
       <c r="Z17" s="18">
         <f t="shared" si="2"/>
-        <v>14532.06</v>
+        <v>15074.71</v>
       </c>
       <c r="AA17" s="18">
         <f t="shared" si="2"/>
-        <v>14562.34</v>
+        <v>15106.12</v>
       </c>
       <c r="AB17" s="18">
         <f t="shared" si="2"/>
-        <v>14592.68</v>
+        <v>15137.59</v>
       </c>
       <c r="AC17" s="18">
         <f t="shared" si="2"/>
-        <v>14623.08</v>
+        <v>15169.13</v>
       </c>
       <c r="AD17" s="18">
         <f t="shared" si="2"/>
-        <v>14653.54</v>
+        <v>15200.73</v>
       </c>
       <c r="AE17" s="18">
         <f t="shared" si="2"/>
-        <v>14684.07</v>
+        <v>15232.4</v>
       </c>
       <c r="AF17" s="18">
         <f t="shared" si="2"/>
-        <v>14714.66</v>
+        <v>15264.13</v>
       </c>
       <c r="AG17" s="18">
         <f t="shared" si="2"/>
-        <v>14745.32</v>
+        <v>15295.93</v>
       </c>
       <c r="AH17" s="18">
         <f t="shared" si="2"/>
-        <v>7761.46</v>
+        <v>8313.2099999999991</v>
       </c>
       <c r="AI17" s="18">
         <f t="shared" si="2"/>
-        <v>7777.63</v>
+        <v>8330.5300000000007</v>
       </c>
       <c r="AJ17" s="18">
         <f t="shared" si="2"/>
-        <v>7793.83</v>
+        <v>8347.89</v>
       </c>
       <c r="AK17" s="18">
         <f t="shared" si="2"/>
-        <v>7810.07</v>
+        <v>8365.2800000000007</v>
       </c>
       <c r="AL17" s="18">
         <f t="shared" si="2"/>
-        <v>7826.34</v>
+        <v>8382.7099999999991</v>
       </c>
       <c r="AM17" s="18">
         <f t="shared" ref="AM17" si="3">AL24</f>
-        <v>7842.64</v>
+        <v>8400.17</v>
       </c>
       <c r="AN17" s="18">
         <f t="shared" ref="AN17" si="4">AM24</f>
-        <v>7858.98</v>
+        <v>8417.67</v>
       </c>
       <c r="AO17" s="18">
         <f t="shared" ref="AO17" si="5">AN24</f>
-        <v>7875.35</v>
+        <v>8435.2099999999991</v>
       </c>
       <c r="AP17" s="18">
         <f t="shared" ref="AP17" si="6">AO24</f>
-        <v>7891.76</v>
+        <v>8452.7800000000007</v>
       </c>
       <c r="AQ17" s="18">
         <f t="shared" ref="AQ17" si="7">AP24</f>
-        <v>7908.2</v>
+        <v>8470.39</v>
       </c>
       <c r="AR17" s="18">
         <f t="shared" ref="AR17" si="8">AQ24</f>
-        <v>7924.68</v>
+        <v>8488.0400000000009</v>
       </c>
       <c r="AS17" s="18">
         <f t="shared" ref="AS17" si="9">AR24</f>
-        <v>7941.19</v>
+        <v>8505.7199999999993</v>
       </c>
       <c r="AT17" s="18">
         <f t="shared" ref="AT17" si="10">AS24</f>
-        <v>943.15</v>
+        <v>1508.86</v>
       </c>
       <c r="AU17" s="18">
         <f t="shared" ref="AU17" si="11">AT24</f>
-        <v>945.11</v>
+        <v>1512</v>
       </c>
       <c r="AV17" s="18">
         <f t="shared" ref="AV17" si="12">AU24</f>
-        <v>947.08</v>
+        <v>1515.15</v>
       </c>
       <c r="AW17" s="18">
         <f t="shared" ref="AW17" si="13">AV24</f>
-        <v>949.05</v>
+        <v>1518.31</v>
       </c>
       <c r="AX17" s="18">
         <f t="shared" ref="AX17" si="14">AW24</f>
-        <v>951.03</v>
+        <v>1521.47</v>
       </c>
       <c r="AY17" s="18">
         <f t="shared" ref="AY17" si="15">AX24</f>
-        <v>953.01</v>
+        <v>1524.64</v>
       </c>
       <c r="AZ17" s="18">
         <f t="shared" ref="AZ17" si="16">AY24</f>
-        <v>955</v>
+        <v>1527.82</v>
       </c>
       <c r="BA17" s="18">
         <f t="shared" ref="BA17" si="17">AZ24</f>
-        <v>956.99</v>
+        <v>1531</v>
       </c>
       <c r="BB17" s="18">
         <f t="shared" ref="BB17" si="18">BA24</f>
-        <v>958.98</v>
+        <v>1534.19</v>
       </c>
       <c r="BC17" s="18">
         <f t="shared" ref="BC17" si="19">BB24</f>
-        <v>960.98</v>
+        <v>1537.39</v>
       </c>
       <c r="BD17" s="18">
         <f t="shared" ref="BD17" si="20">BC24</f>
-        <v>962.98</v>
+        <v>1540.59</v>
       </c>
       <c r="BE17" s="18">
         <f t="shared" ref="BE17" si="21">BD24</f>
-        <v>964.99</v>
+        <v>1543.8</v>
       </c>
       <c r="BF17" s="18">
         <f t="shared" ref="BF17" si="22">BE24</f>
-        <v>5977.42</v>
+        <v>6557.43</v>
       </c>
       <c r="BG17" s="18">
         <f t="shared" ref="BG17" si="23">BF24</f>
-        <v>11000.29</v>
+        <v>11581.51</v>
       </c>
       <c r="BH17" s="18">
         <f t="shared" ref="BH17" si="24">BG24</f>
-        <v>16033.62</v>
+        <v>16616.05</v>
       </c>
       <c r="BI17" s="18">
         <f t="shared" ref="BI17" si="25">BH24</f>
-        <v>21077.439999999999</v>
+        <v>21661.08</v>
       </c>
       <c r="BJ17" s="18">
         <f t="shared" ref="BJ17" si="26">BI24</f>
-        <v>26131.77</v>
+        <v>26716.62</v>
       </c>
     </row>
     <row r="18" spans="1:62" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -14953,7 +14959,7 @@
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
-      <c r="I19" s="11">
+      <c r="I19" s="22">
         <v>4010</v>
       </c>
       <c r="J19" s="11">
@@ -15334,219 +15340,219 @@
       </c>
       <c r="I23">
         <f>SUMIF(Table143911[Type],"Income",Table143911[Jul-25])-SUMIF(Table143911[Type],"Expense",Table143911[Jul-25])</f>
-        <v>22848.19</v>
+        <v>23371.95</v>
       </c>
       <c r="J23">
         <f>SUMIF(Table143911[Type],"Income",Table143911[Aug-25])-SUMIF(Table143911[Type],"Expense",Table143911[Aug-25])</f>
-        <v>23885.79</v>
+        <v>24410.639999999999</v>
       </c>
       <c r="K23">
         <f>SUMIF(Table143911[Type],"Income",Table143911[Sep-25])-SUMIF(Table143911[Type],"Expense",Table143911[Sep-25])</f>
-        <v>24925.55</v>
+        <v>25451.5</v>
       </c>
       <c r="L23">
         <f>SUMIF(Table143911[Type],"Income",Table143911[Oct-25])-SUMIF(Table143911[Type],"Expense",Table143911[Oct-25])</f>
-        <v>25967.48</v>
+        <v>26494.52</v>
       </c>
       <c r="M23">
         <f>SUMIF(Table143911[Type],"Income",Table143911[Nov-25])-SUMIF(Table143911[Type],"Expense",Table143911[Nov-25])</f>
-        <v>27011.58</v>
+        <v>27539.72</v>
       </c>
       <c r="N23">
         <f>SUMIF(Table143911[Type],"Income",Table143911[Dec-25])-SUMIF(Table143911[Type],"Expense",Table143911[Dec-25])</f>
-        <v>28057.85</v>
+        <v>28587.09</v>
       </c>
       <c r="O23">
         <f>SUMIF(Table143911[Type],"Income",Table143911[Jan-26])-SUMIF(Table143911[Type],"Expense",Table143911[Jan-26])</f>
-        <v>21116.300000000003</v>
+        <v>21646.65</v>
       </c>
       <c r="P23">
         <f>SUMIF(Table143911[Type],"Income",Table143911[Feb-26])-SUMIF(Table143911[Type],"Expense",Table143911[Feb-26])</f>
-        <v>21160.29</v>
+        <v>21691.75</v>
       </c>
       <c r="Q23">
         <f>SUMIF(Table143911[Type],"Income",Table143911[Mar-26])-SUMIF(Table143911[Type],"Expense",Table143911[Mar-26])</f>
-        <v>21204.37</v>
+        <v>21736.94</v>
       </c>
       <c r="R23">
         <f>SUMIF(Table143911[Type],"Income",Table143911[Apr-26])-SUMIF(Table143911[Type],"Expense",Table143911[Apr-26])</f>
-        <v>21248.55</v>
+        <v>21782.23</v>
       </c>
       <c r="S23">
         <f>SUMIF(Table143911[Type],"Income",Table143911[May-26])-SUMIF(Table143911[Type],"Expense",Table143911[May-26])</f>
-        <v>21292.82</v>
+        <v>21827.61</v>
       </c>
       <c r="T23">
         <f>SUMIF(Table143911[Type],"Income",Table143911[Jun-26])-SUMIF(Table143911[Type],"Expense",Table143911[Jun-26])</f>
-        <v>21337.18</v>
+        <v>21873.08</v>
       </c>
       <c r="U23">
         <f>SUMIF(Table143911[Type],"Income",Table143911[Jul-26])-SUMIF(Table143911[Type],"Expense",Table143911[Jul-26])</f>
-        <v>14381.630000000001</v>
+        <v>14918.650000000001</v>
       </c>
       <c r="V23">
         <f>SUMIF(Table143911[Type],"Income",Table143911[Aug-26])-SUMIF(Table143911[Type],"Expense",Table143911[Aug-26])</f>
-        <v>14411.59</v>
+        <v>14949.73</v>
       </c>
       <c r="W23">
         <f>SUMIF(Table143911[Type],"Income",Table143911[Sep-26])-SUMIF(Table143911[Type],"Expense",Table143911[Sep-26])</f>
-        <v>14441.61</v>
+        <v>14980.879999999997</v>
       </c>
       <c r="X23">
         <f>SUMIF(Table143911[Type],"Income",Table143911[Oct-26])-SUMIF(Table143911[Type],"Expense",Table143911[Oct-26])</f>
-        <v>14471.7</v>
+        <v>15012.09</v>
       </c>
       <c r="Y23">
         <f>SUMIF(Table143911[Type],"Income",Table143911[Nov-26])-SUMIF(Table143911[Type],"Expense",Table143911[Nov-26])</f>
-        <v>14501.849999999999</v>
+        <v>15043.370000000003</v>
       </c>
       <c r="Z23">
         <f>SUMIF(Table143911[Type],"Income",Table143911[Dec-26])-SUMIF(Table143911[Type],"Expense",Table143911[Dec-26])</f>
-        <v>14532.059999999998</v>
+        <v>15074.71</v>
       </c>
       <c r="AA23">
         <f>SUMIF(Table143911[Type],"Income",Table143911[Jan-27])-SUMIF(Table143911[Type],"Expense",Table143911[Jan-27])</f>
-        <v>14562.34</v>
+        <v>15106.120000000003</v>
       </c>
       <c r="AB23">
         <f>SUMIF(Table143911[Type],"Income",Table143911[Feb-27])-SUMIF(Table143911[Type],"Expense",Table143911[Feb-27])</f>
-        <v>14592.68</v>
+        <v>15137.59</v>
       </c>
       <c r="AC23">
         <f>SUMIF(Table143911[Type],"Income",Table143911[Mar-27])-SUMIF(Table143911[Type],"Expense",Table143911[Mar-27])</f>
-        <v>14623.080000000002</v>
+        <v>15169.129999999997</v>
       </c>
       <c r="AD23">
         <f>SUMIF(Table143911[Type],"Income",Table143911[Apr-27])-SUMIF(Table143911[Type],"Expense",Table143911[Apr-27])</f>
-        <v>14653.54</v>
+        <v>15200.73</v>
       </c>
       <c r="AE23">
         <f>SUMIF(Table143911[Type],"Income",Table143911[May-27])-SUMIF(Table143911[Type],"Expense",Table143911[May-27])</f>
-        <v>14684.07</v>
+        <v>15232.400000000001</v>
       </c>
       <c r="AF23">
         <f>SUMIF(Table143911[Type],"Income",Table143911[Jun-27])-SUMIF(Table143911[Type],"Expense",Table143911[Jun-27])</f>
-        <v>14714.66</v>
+        <v>15264.129999999997</v>
       </c>
       <c r="AG23">
         <f>SUMIF(Table143911[Type],"Income",Table143911[Jul-27])-SUMIF(Table143911[Type],"Expense",Table143911[Jul-27])</f>
-        <v>7745.32</v>
+        <v>8295.93</v>
       </c>
       <c r="AH23">
         <f>SUMIF(Table143911[Type],"Income",Table143911[Aug-27])-SUMIF(Table143911[Type],"Expense",Table143911[Aug-27])</f>
-        <v>7761.4599999999991</v>
+        <v>8313.2099999999991</v>
       </c>
       <c r="AI23">
         <f>SUMIF(Table143911[Type],"Income",Table143911[Sep-27])-SUMIF(Table143911[Type],"Expense",Table143911[Sep-27])</f>
-        <v>7777.630000000001</v>
+        <v>8330.5300000000007</v>
       </c>
       <c r="AJ23">
         <f>SUMIF(Table143911[Type],"Income",Table143911[Oct-27])-SUMIF(Table143911[Type],"Expense",Table143911[Oct-27])</f>
-        <v>7793.83</v>
+        <v>8347.89</v>
       </c>
       <c r="AK23">
         <f>SUMIF(Table143911[Type],"Income",Table143911[Nov-27])-SUMIF(Table143911[Type],"Expense",Table143911[Nov-27])</f>
-        <v>7810.07</v>
+        <v>8365.2800000000007</v>
       </c>
       <c r="AL23">
         <f>SUMIF(Table143911[Type],"Income",Table143911[Dec-27])-SUMIF(Table143911[Type],"Expense",Table143911[Dec-27])</f>
-        <v>7826.34</v>
+        <v>8382.7099999999991</v>
       </c>
       <c r="AM23">
         <f>SUMIF(Table143911[Type], "Income",Table143911[Jan-28])-SUMIF(Table143911[Type], "Expense",Table143911[Jan-28])</f>
-        <v>7842.6399999999994</v>
+        <v>8400.17</v>
       </c>
       <c r="AN23">
         <f>SUMIF(Table143911[Type], "Income",Table143911[Feb-28])-SUMIF(Table143911[Type], "Expense",Table143911[Feb-28])</f>
-        <v>7858.98</v>
+        <v>8417.67</v>
       </c>
       <c r="AO23">
         <f>SUMIF(Table143911[Type], "Income",Table143911[Mar-28])-SUMIF(Table143911[Type], "Expense",Table143911[Mar-28])</f>
-        <v>7875.35</v>
+        <v>8435.2099999999991</v>
       </c>
       <c r="AP23">
         <f>SUMIF(Table143911[Type], "Income",Table143911[Apr-28])-SUMIF(Table143911[Type], "Expense",Table143911[Apr-28])</f>
-        <v>7891.76</v>
+        <v>8452.7800000000007</v>
       </c>
       <c r="AQ23">
         <f>SUMIF(Table143911[Type], "Income",Table143911[May-28])-SUMIF(Table143911[Type], "Expense",Table143911[May-28])</f>
-        <v>7908.2000000000007</v>
+        <v>8470.39</v>
       </c>
       <c r="AR23">
         <f>SUMIF(Table143911[Type], "Income",Table143911[Jun-28])-SUMIF(Table143911[Type], "Expense",Table143911[Jun-28])</f>
-        <v>7924.68</v>
+        <v>8488.0400000000009</v>
       </c>
       <c r="AS23">
         <f>SUMIF(Table143911[Type], "Income",Table143911[Jul-28])-SUMIF(Table143911[Type], "Expense",Table143911[Jul-28])</f>
-        <v>941.18999999999869</v>
+        <v>1505.7199999999993</v>
       </c>
       <c r="AT23">
         <f>SUMIF(Table143911[Type], "Income",Table143911[Aug-28])-SUMIF(Table143911[Type], "Expense",Table143911[Aug-28])</f>
-        <v>943.14999999999964</v>
+        <v>1508.8599999999997</v>
       </c>
       <c r="AU23">
         <f>SUMIF(Table143911[Type], "Income",Table143911[Sep-28])-SUMIF(Table143911[Type], "Expense",Table143911[Sep-28])</f>
-        <v>945.10999999999967</v>
+        <v>1512</v>
       </c>
       <c r="AV23">
         <f>SUMIF(Table143911[Type], "Income",Table143911[Oct-28])-SUMIF(Table143911[Type], "Expense",Table143911[Oct-28])</f>
-        <v>947.07999999999993</v>
+        <v>1515.1499999999996</v>
       </c>
       <c r="AW23">
         <f>SUMIF(Table143911[Type], "Income",Table143911[Nov-28])-SUMIF(Table143911[Type], "Expense",Table143911[Nov-28])</f>
-        <v>949.05000000000018</v>
+        <v>1518.3099999999995</v>
       </c>
       <c r="AX23">
         <f>SUMIF(Table143911[Type], "Income",Table143911[Dec-28])-SUMIF(Table143911[Type], "Expense",Table143911[Dec-28])</f>
-        <v>951.02999999999975</v>
+        <v>1521.4700000000003</v>
       </c>
       <c r="AY23">
         <f>SUMIF(Table143911[Type], "Income",Table143911[Jan-29])-SUMIF(Table143911[Type], "Expense",Table143911[Jan-29])</f>
-        <v>953.01000000000022</v>
+        <v>1524.6400000000003</v>
       </c>
       <c r="AZ23">
         <f>SUMIF(Table143911[Type], "Income",Table143911[Feb-29])-SUMIF(Table143911[Type], "Expense",Table143911[Feb-29])</f>
-        <v>955</v>
+        <v>1527.8199999999997</v>
       </c>
       <c r="BA23">
         <f>SUMIF(Table143911[Type], "Income",Table143911[Mar-29])-SUMIF(Table143911[Type], "Expense",Table143911[Mar-29])</f>
-        <v>956.98999999999978</v>
+        <v>1531</v>
       </c>
       <c r="BB23">
         <f>SUMIF(Table143911[Type], "Income",Table143911[Apr-29])-SUMIF(Table143911[Type], "Expense",Table143911[Apr-29])</f>
-        <v>958.97999999999956</v>
+        <v>1534.1900000000005</v>
       </c>
       <c r="BC23">
         <f>SUMIF(Table143911[Type], "Income",Table143911[May-29])-SUMIF(Table143911[Type], "Expense",Table143911[May-29])</f>
-        <v>960.97999999999956</v>
+        <v>1537.3900000000003</v>
       </c>
       <c r="BD23">
         <f>SUMIF(Table143911[Type], "Income",Table143911[Jun-29])-SUMIF(Table143911[Type], "Expense",Table143911[Jun-29])</f>
-        <v>962.97999999999956</v>
+        <v>1540.5900000000001</v>
       </c>
       <c r="BE23">
         <f>SUMIF(Table143911[Type], "Income",Table143911[Jul-29])-SUMIF(Table143911[Type], "Expense",Table143911[Jul-29])</f>
-        <v>5964.99</v>
+        <v>6543.8</v>
       </c>
       <c r="BF23">
         <f>SUMIF(Table143911[Type], "Income",Table143911[Aug-29])-SUMIF(Table143911[Type], "Expense",Table143911[Aug-29])</f>
-        <v>10977.42</v>
+        <v>11557.43</v>
       </c>
       <c r="BG23">
         <f>SUMIF(Table143911[Type], "Income",Table143911[Sep-29])-SUMIF(Table143911[Type], "Expense",Table143911[Sep-29])</f>
-        <v>16000.29</v>
+        <v>16581.510000000002</v>
       </c>
       <c r="BH23">
         <f>SUMIF(Table143911[Type], "Income",Table143911[Oct-29])-SUMIF(Table143911[Type], "Expense",Table143911[Oct-29])</f>
-        <v>21033.620000000003</v>
+        <v>21616.05</v>
       </c>
       <c r="BI23">
         <f>SUMIF(Table143911[Type], "Income",Table143911[Nov-29])-SUMIF(Table143911[Type], "Expense",Table143911[Nov-29])</f>
-        <v>26077.439999999999</v>
+        <v>26661.08</v>
       </c>
       <c r="BJ23">
         <f>SUMIF(Table143911[Type], "Income",Table143911[Dec-29])-SUMIF(Table143911[Type], "Expense",Table143911[Dec-29])</f>
-        <v>31131.77</v>
+        <v>31716.62</v>
       </c>
     </row>
     <row r="24" spans="1:62" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -15579,219 +15585,219 @@
       </c>
       <c r="I24" s="1">
         <f>ROUND(Table143911[[#Totals],[Jul-25]]*$B$3,2)</f>
-        <v>22895.79</v>
+        <v>23420.639999999999</v>
       </c>
       <c r="J24" s="1">
         <f>ROUND(Table143911[[#Totals],[Aug-25]]*$B$3,2)</f>
-        <v>23935.55</v>
+        <v>24461.5</v>
       </c>
       <c r="K24" s="1">
         <f>ROUND(Table143911[[#Totals],[Sep-25]]*$B$3,2)</f>
-        <v>24977.48</v>
+        <v>25504.52</v>
       </c>
       <c r="L24" s="1">
         <f>ROUND(Table143911[[#Totals],[Oct-25]]*$B$3,2)</f>
-        <v>26021.58</v>
+        <v>26549.72</v>
       </c>
       <c r="M24" s="1">
         <f>ROUND(Table143911[[#Totals],[Nov-25]]*$B$3,2)</f>
-        <v>27067.85</v>
+        <v>27597.09</v>
       </c>
       <c r="N24" s="1">
         <f>ROUND(Table143911[[#Totals],[Dec-25]]*$B$3,2)</f>
-        <v>28116.3</v>
+        <v>28646.65</v>
       </c>
       <c r="O24" s="1">
         <f>ROUND(Table143911[[#Totals],[Jan-26]]*$B$3,2)</f>
-        <v>21160.29</v>
+        <v>21691.75</v>
       </c>
       <c r="P24" s="1">
         <f>ROUND(Table143911[[#Totals],[Feb-26]]*$B$3,2)</f>
-        <v>21204.37</v>
+        <v>21736.94</v>
       </c>
       <c r="Q24" s="1">
         <f>ROUND(Table143911[[#Totals],[Mar-26]]*$B$3,2)</f>
-        <v>21248.55</v>
+        <v>21782.23</v>
       </c>
       <c r="R24" s="1">
         <f>ROUND(Table143911[[#Totals],[Apr-26]]*$B$3,2)</f>
-        <v>21292.82</v>
+        <v>21827.61</v>
       </c>
       <c r="S24" s="1">
         <f>ROUND(Table143911[[#Totals],[May-26]]*$B$3,2)</f>
-        <v>21337.18</v>
+        <v>21873.08</v>
       </c>
       <c r="T24" s="1">
         <f>ROUND(Table143911[[#Totals],[Jun-26]]*$B$3,2)</f>
-        <v>21381.63</v>
+        <v>21918.65</v>
       </c>
       <c r="U24" s="1">
         <f>ROUND(Table143911[[#Totals],[Jul-26]]*$B$3,2)</f>
-        <v>14411.59</v>
+        <v>14949.73</v>
       </c>
       <c r="V24" s="1">
         <f>ROUND(Table143911[[#Totals],[Aug-26]]*$B$3,2)</f>
-        <v>14441.61</v>
+        <v>14980.88</v>
       </c>
       <c r="W24" s="1">
         <f>ROUND(Table143911[[#Totals],[Sep-26]]*$B$3,2)</f>
-        <v>14471.7</v>
+        <v>15012.09</v>
       </c>
       <c r="X24" s="1">
         <f>ROUND(Table143911[[#Totals],[Oct-26]]*$B$3,2)</f>
-        <v>14501.85</v>
+        <v>15043.37</v>
       </c>
       <c r="Y24" s="1">
         <f>ROUND(Table143911[[#Totals],[Nov-26]]*$B$3,2)</f>
-        <v>14532.06</v>
+        <v>15074.71</v>
       </c>
       <c r="Z24" s="1">
         <f>ROUND(Table143911[[#Totals],[Dec-26]]*$B$3,2)</f>
-        <v>14562.34</v>
+        <v>15106.12</v>
       </c>
       <c r="AA24" s="1">
         <f>ROUND(Table143911[[#Totals],[Jan-27]]*$B$3,2)</f>
-        <v>14592.68</v>
+        <v>15137.59</v>
       </c>
       <c r="AB24" s="1">
         <f>ROUND(Table143911[[#Totals],[Feb-27]]*$B$3,2)</f>
-        <v>14623.08</v>
+        <v>15169.13</v>
       </c>
       <c r="AC24" s="1">
         <f>ROUND(Table143911[[#Totals],[Mar-27]]*$B$3,2)</f>
-        <v>14653.54</v>
+        <v>15200.73</v>
       </c>
       <c r="AD24" s="1">
         <f>ROUND(Table143911[[#Totals],[Apr-27]]*$B$3,2)</f>
-        <v>14684.07</v>
+        <v>15232.4</v>
       </c>
       <c r="AE24" s="1">
         <f>ROUND(Table143911[[#Totals],[May-27]]*$B$3,2)</f>
-        <v>14714.66</v>
+        <v>15264.13</v>
       </c>
       <c r="AF24" s="1">
         <f>ROUND(Table143911[[#Totals],[Jun-27]]*$B$3,2)</f>
-        <v>14745.32</v>
+        <v>15295.93</v>
       </c>
       <c r="AG24" s="1">
         <f>ROUND(Table143911[[#Totals],[Jul-27]]*$B$3,2)</f>
-        <v>7761.46</v>
+        <v>8313.2099999999991</v>
       </c>
       <c r="AH24" s="1">
         <f>ROUND(Table143911[[#Totals],[Aug-27]]*$B$3,2)</f>
-        <v>7777.63</v>
+        <v>8330.5300000000007</v>
       </c>
       <c r="AI24" s="1">
         <f>ROUND(Table143911[[#Totals],[Sep-27]]*$B$3,2)</f>
-        <v>7793.83</v>
+        <v>8347.89</v>
       </c>
       <c r="AJ24" s="1">
         <f>ROUND(Table143911[[#Totals],[Oct-27]]*$B$3,2)</f>
-        <v>7810.07</v>
+        <v>8365.2800000000007</v>
       </c>
       <c r="AK24" s="1">
         <f>ROUND(Table143911[[#Totals],[Nov-27]]*$B$3,2)</f>
-        <v>7826.34</v>
+        <v>8382.7099999999991</v>
       </c>
       <c r="AL24" s="1">
         <f>ROUND(Table143911[[#Totals],[Dec-27]]*$B$3,2)</f>
-        <v>7842.64</v>
+        <v>8400.17</v>
       </c>
       <c r="AM24">
         <f>ROUND(Table143911[[#Totals],[Jan-28]]*$B$3,2)</f>
-        <v>7858.98</v>
+        <v>8417.67</v>
       </c>
       <c r="AN24">
         <f>ROUND(Table143911[[#Totals],[Feb-28]]*$B$3,2)</f>
-        <v>7875.35</v>
+        <v>8435.2099999999991</v>
       </c>
       <c r="AO24">
         <f>ROUND(Table143911[[#Totals],[Mar-28]]*$B$3,2)</f>
-        <v>7891.76</v>
+        <v>8452.7800000000007</v>
       </c>
       <c r="AP24">
         <f>ROUND(Table143911[[#Totals],[Apr-28]]*$B$3,2)</f>
-        <v>7908.2</v>
+        <v>8470.39</v>
       </c>
       <c r="AQ24">
         <f>ROUND(Table143911[[#Totals],[May-28]]*$B$3,2)</f>
-        <v>7924.68</v>
+        <v>8488.0400000000009</v>
       </c>
       <c r="AR24">
         <f>ROUND(Table143911[[#Totals],[Jun-28]]*$B$3,2)</f>
-        <v>7941.19</v>
+        <v>8505.7199999999993</v>
       </c>
       <c r="AS24">
         <f>ROUND(Table143911[[#Totals],[Jul-28]]*$B$3,2)</f>
-        <v>943.15</v>
+        <v>1508.86</v>
       </c>
       <c r="AT24">
         <f>ROUND(Table143911[[#Totals],[Aug-28]]*$B$3,2)</f>
-        <v>945.11</v>
+        <v>1512</v>
       </c>
       <c r="AU24">
         <f>ROUND(Table143911[[#Totals],[Sep-28]]*$B$3,2)</f>
-        <v>947.08</v>
+        <v>1515.15</v>
       </c>
       <c r="AV24">
         <f>ROUND(Table143911[[#Totals],[Oct-28]]*$B$3,2)</f>
-        <v>949.05</v>
+        <v>1518.31</v>
       </c>
       <c r="AW24">
         <f>ROUND(Table143911[[#Totals],[Nov-28]]*$B$3,2)</f>
-        <v>951.03</v>
+        <v>1521.47</v>
       </c>
       <c r="AX24">
         <f>ROUND(Table143911[[#Totals],[Dec-28]]*$B$3,2)</f>
-        <v>953.01</v>
+        <v>1524.64</v>
       </c>
       <c r="AY24">
         <f>ROUND(Table143911[[#Totals],[Jan-29]]*$B$3,2)</f>
-        <v>955</v>
+        <v>1527.82</v>
       </c>
       <c r="AZ24">
         <f>ROUND(Table143911[[#Totals],[Feb-29]]*$B$3,2)</f>
-        <v>956.99</v>
+        <v>1531</v>
       </c>
       <c r="BA24">
         <f>ROUND(Table143911[[#Totals],[Mar-29]]*$B$3,2)</f>
-        <v>958.98</v>
+        <v>1534.19</v>
       </c>
       <c r="BB24">
         <f>ROUND(Table143911[[#Totals],[Apr-29]]*$B$3,2)</f>
-        <v>960.98</v>
+        <v>1537.39</v>
       </c>
       <c r="BC24">
         <f>ROUND(Table143911[[#Totals],[May-29]]*$B$3,2)</f>
-        <v>962.98</v>
+        <v>1540.59</v>
       </c>
       <c r="BD24">
         <f>ROUND(Table143911[[#Totals],[Jun-29]]*$B$3,2)</f>
-        <v>964.99</v>
+        <v>1543.8</v>
       </c>
       <c r="BE24">
         <f>ROUND(Table143911[[#Totals],[Jul-29]]*$B$3,2)</f>
-        <v>5977.42</v>
+        <v>6557.43</v>
       </c>
       <c r="BF24">
         <f>ROUND(Table143911[[#Totals],[Aug-29]]*$B$3,2)</f>
-        <v>11000.29</v>
+        <v>11581.51</v>
       </c>
       <c r="BG24">
         <f>ROUND(Table143911[[#Totals],[Sep-29]]*$B$3,2)</f>
-        <v>16033.62</v>
+        <v>16616.05</v>
       </c>
       <c r="BH24">
         <f>ROUND(Table143911[[#Totals],[Oct-29]]*$B$3,2)</f>
-        <v>21077.439999999999</v>
+        <v>21661.08</v>
       </c>
       <c r="BI24">
         <f>ROUND(Table143911[[#Totals],[Nov-29]]*$B$3,2)</f>
-        <v>26131.77</v>
+        <v>26716.62</v>
       </c>
       <c r="BJ24">
         <f>ROUND(Table143911[[#Totals],[Dec-29]]*$B$3,2)</f>
-        <v>31196.63</v>
+        <v>31782.7</v>
       </c>
     </row>
     <row r="25" spans="1:62" x14ac:dyDescent="0.2">
@@ -15802,6 +15808,9 @@
         <v>80</v>
       </c>
       <c r="G25" t="s">
+        <v>80</v>
+      </c>
+      <c r="I25" t="s">
         <v>80</v>
       </c>
     </row>

</xml_diff>